<commit_message>
change xpath and update test script and create new methods for handle date picker
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -3,16 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FBD338-0920-410B-9696-53FD0001584E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0832F9A0-1E3E-4279-88AA-3D5CB2877A3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateOwn Test Data" sheetId="1" r:id="rId1"/>
+    <sheet name="AddAchievement Test Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Create Activity Error Msg Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>Cycling</t>
   </si>
@@ -67,21 +69,64 @@
     <t>1111</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
+    <t>AchievementDropDownValue</t>
+  </si>
+  <si>
+    <t>ProficiencyLevelDropDown</t>
+  </si>
+  <si>
+    <t>Cricket</t>
+  </si>
+  <si>
+    <t>Level completion</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>First Prize</t>
+  </si>
+  <si>
+    <t>ACHIEVEMENT ADDED &amp; APPROVED!</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>DateOfMonth</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>Enter Activity Title</t>
+  </si>
+  <si>
+    <t>Enter Activity Description</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,15 +155,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,18 +445,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.109375"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.109375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.6640625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="29.6640625"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -432,45 +480,42 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s" s="0">
-        <v>15</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -478,4 +523,168 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99C60738-FDC7-49E4-8AB9-64CD81403A94}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{DBE594B6-F8A6-40AB-8AD9-30F4E2938BF4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE76969-77BE-4CF5-B26D-565FB05E9A5F}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Conditions use for different activity
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0832F9A0-1E3E-4279-88AA-3D5CB2877A3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9F98FB-7C79-48C5-B861-4E9CB297A2EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateOwn Test Data" sheetId="1" r:id="rId1"/>
-    <sheet name="AddAchievement Test Data" sheetId="2" r:id="rId2"/>
-    <sheet name="Create Activity Error Msg Data" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="AddAchievement Test Data" sheetId="2" r:id="rId3"/>
+    <sheet name="Create Activity Error Msg Data" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="49">
   <si>
     <t>Cycling</t>
   </si>
@@ -109,6 +110,66 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>activityType</t>
+  </si>
+  <si>
+    <t>Once</t>
+  </si>
+  <si>
+    <t>timeRequired</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>completeWithin</t>
+  </si>
+  <si>
+    <t>expectedActivityCreatedMsg</t>
+  </si>
+  <si>
+    <t>YAY! IT'S ASSIGNED</t>
+  </si>
+  <si>
+    <t>DAY</t>
+  </si>
+  <si>
+    <t>expectedAssignedActivityMsg</t>
+  </si>
+  <si>
+    <t>points</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>statusOfActivity</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>expectedToastMsg</t>
+  </si>
+  <si>
+    <t>Activity Deleted Successfully</t>
+  </si>
+  <si>
+    <t>endAfterDays</t>
+  </si>
+  <si>
+    <t>Every Day</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>16</t>
   </si>
 </sst>
 </file>
@@ -445,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,9 +518,16 @@
     <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" customWidth="1"/>
+    <col min="12" max="12" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -476,10 +544,37 @@
         <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -498,8 +593,35 @@
       <c r="F2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -517,6 +639,33 @@
       </c>
       <c r="F3" t="s">
         <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O3" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -526,6 +675,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A25A53-32F2-4315-9A12-DA52E7A6ED94}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99C60738-FDC7-49E4-8AB9-64CD81403A94}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -605,12 +789,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE76969-77BE-4CF5-B26D-565FB05E9A5F}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>